<commit_message>
temporary save updates of application
</commit_message>
<xml_diff>
--- a/data/sharepoint_docs/Construction-Estimate/estimate_MO0008_船橋物流センター北_v1.1.xlsx
+++ b/data/sharepoint_docs/Construction-Estimate/estimate_MO0008_船橋物流センター北_v1.1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shota.hayashida\Downloads\サンプル報告書\Construction-Estimate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shota.hayashida\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B130284-EDC0-4702-B9D9-C683E1BC576B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F15372F-06A3-4EB5-80EA-B77C69E39410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -376,10 +376,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>台風による建物の大規模損傷（安全確認のため屋上立入禁止）のため、工事を一時中断し、工期を【着工 2025/10/10／竣工 2025/12/05】から未定へ変更（復旧工事・安全確認の完了待ち／工程再編）</t>
-    <rPh sb="75" eb="77">
-      <t>ミテイ</t>
-    </rPh>
+    <t>台風による建物の大規模損傷（安全確認のため屋上立入禁止）のため、工事を一時中断とする（復旧工事・安全確認の完了待ち／工程再編）</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1395,8 +1392,8 @@
   </sheetPr>
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51:H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.4"/>

</xml_diff>